<commit_message>
add outcome definition (#16)
</commit_message>
<xml_diff>
--- a/data/en/outcome_table.xlsx
+++ b/data/en/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kansenkloof_NL/data/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D742EE63-D015-B340-9EE9-4986DEFCD36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C20CFA-A1BB-BF4C-B058-5095064F4F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -1692,34 +1692,34 @@
     <t>Zwijndrecht</t>
   </si>
   <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>Test 6</t>
-  </si>
-  <si>
-    <t>Test 7</t>
-  </si>
-  <si>
-    <t>Test 8</t>
-  </si>
-  <si>
-    <t>Test 9</t>
-  </si>
-  <si>
-    <t>Test 10</t>
+    <t>refers to the percentage of classmates in the final grade of primary school with low-income parents.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school with high-income parents.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school whose parents are both born abroad.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school with at least a moderate test score.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school with at least a high test score.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school with a very high test score.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school who met the target level for reading comprehension.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school who met the target level for mathematics.</t>
+  </si>
+  <si>
+    <t>refers to the percentage of classmates in the final grade of primary school who met the target level for grammar and writing.</t>
+  </si>
+  <si>
+    <t>refers to the average class size in the final grade of primary school.</t>
   </si>
 </sst>
 </file>
@@ -1932,9 +1932,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1972,7 +1972,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2078,7 +2078,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2220,7 +2220,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>